<commit_message>
changed present weather dtype to int32 (int64 not supportedin netcdf4)
</commit_message>
<xml_diff>
--- a/specific_variables/present-weather.xlsx
+++ b/specific_variables/present-weather.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/specific_variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A77A46-2675-E04F-9FA9-B0D7A5E7CD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F09CF1-5F81-8E4E-AB3D-CECBD26304F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="600" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables-specific" sheetId="2" r:id="rId1"/>
@@ -115,9 +115,6 @@
     <t>time: point</t>
   </si>
   <si>
-    <t>int64</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>0b, 1b, 2b</t>
+  </si>
+  <si>
+    <t>int32</t>
   </si>
 </sst>
 </file>
@@ -572,7 +572,7 @@
   <dimension ref="A1:D983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -605,7 +605,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12" customHeight="1">
@@ -645,7 +645,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="12" customHeight="1">
@@ -653,7 +653,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="12" customHeight="1">
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="12" customHeight="1">
@@ -783,7 +783,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="12" customHeight="1">
@@ -894,7 +894,7 @@
         <v>14</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="12" customHeight="1">
@@ -903,7 +903,7 @@
         <v>15</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12" customHeight="1">

</xml_diff>